<commit_message>
<wip> started global sensitivity analysis...
</commit_message>
<xml_diff>
--- a/data/infographic/regional_stats.xlsx
+++ b/data/infographic/regional_stats.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioxfordnexus-my.sharepoint.com/personal/hert5230_ox_ac_uk/Documents/local/OMS/data/infographic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="120" documentId="8_{94A55717-DA04-3C45-BBD6-1172C2735F1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD5858BA-0328-9244-9385-E09EFB66C02B}"/>
+  <xr:revisionPtr revIDLastSave="232" documentId="8_{94A55717-DA04-3C45-BBD6-1172C2735F1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{14D7D9C2-C50D-7947-A521-4E84A1CB4C63}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="680" windowWidth="28040" windowHeight="17420" activeTab="3" xr2:uid="{F5D7289B-2485-3448-A2C6-D1F227A3254D}"/>
+    <workbookView xWindow="940" yWindow="760" windowWidth="28040" windowHeight="17420" activeTab="4" xr2:uid="{F5D7289B-2485-3448-A2C6-D1F227A3254D}"/>
   </bookViews>
   <sheets>
     <sheet name="population" sheetId="3" r:id="rId1"/>
     <sheet name="fuel mix pie charts" sheetId="1" r:id="rId2"/>
     <sheet name="elec consumption per capita" sheetId="2" r:id="rId3"/>
     <sheet name="elec gen per capita" sheetId="4" r:id="rId4"/>
+    <sheet name="elec supply" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="42">
   <si>
     <t>Country</t>
   </si>
@@ -143,15 +144,63 @@
   <si>
     <t>Annual electricity generation per capita: kWh/capita</t>
   </si>
+  <si>
+    <t>Annual electricity generation: TWh</t>
+  </si>
+  <si>
+    <t>https://openknowledge.worldbank.org/bitstream/handle/10986/19226/396950GZ0Energ1white0cover01PUBLIC1.pdf?sequence=1&amp;isAllowed=y</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Pie chart percentages</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Percentage relative to max supply (Egypt)</t>
+  </si>
+  <si>
+    <t>Percentage relative to max supply (Israel)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -174,18 +223,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Per cent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -8604,8 +8664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D3825E3-5CC6-1044-BA2B-5232B6AA19C0}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8972,4 +9032,573 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6090FAF4-1C62-3F46-8C62-45614A747C6E}">
+  <dimension ref="A1:L32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="40.83203125" customWidth="1"/>
+    <col min="3" max="3" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2001</v>
+      </c>
+      <c r="B4" s="3">
+        <f>VLOOKUP(A4,population!A2:E33,5)*VLOOKUP(A4,'elec gen per capita'!A3:E22,2)*0.00000001</f>
+        <v>35.499999999999744</v>
+      </c>
+      <c r="C4" s="3">
+        <f>VLOOKUP(A4,population!A2:E33,3)*VLOOKUP(A4,'elec gen per capita'!A3:E22,3)*0.00000001</f>
+        <v>7511.5337350255741</v>
+      </c>
+      <c r="D4" s="3">
+        <f>VLOOKUP(A4,population!A2:E33,4)*VLOOKUP(A4,'elec gen per capita'!A3:E22,4)*0.00000001</f>
+        <v>43950.999999999993</v>
+      </c>
+      <c r="E4" s="3">
+        <f>VLOOKUP(A4,population!A2:E33,2)*VLOOKUP(A4,'elec gen per capita'!A3:E22,5)*0.00000001</f>
+        <v>76807.999999999578</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2002</v>
+      </c>
+      <c r="B5" s="3">
+        <f>VLOOKUP(A5,population!A3:E34,5)*VLOOKUP(A5,'elec gen per capita'!A4:E23,2)*0.00000001</f>
+        <v>149.29999999999978</v>
+      </c>
+      <c r="C5" s="3">
+        <f>VLOOKUP(A5,population!A3:E34,3)*VLOOKUP(A5,'elec gen per capita'!A4:E23,3)*0.00000001</f>
+        <v>7688.8640346169313</v>
+      </c>
+      <c r="D5" s="3">
+        <f>VLOOKUP(A5,population!A3:E34,4)*VLOOKUP(A5,'elec gen per capita'!A4:E23,4)*0.00000001</f>
+        <v>45499.999999999964</v>
+      </c>
+      <c r="E5" s="3">
+        <f>VLOOKUP(A5,population!A3:E34,2)*VLOOKUP(A5,'elec gen per capita'!A4:E23,5)*0.00000001</f>
+        <v>85945.999999999927</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2003</v>
+      </c>
+      <c r="B6" s="3">
+        <f>VLOOKUP(A6,population!A4:E35,5)*VLOOKUP(A6,'elec gen per capita'!A5:E24,2)*0.00000001</f>
+        <v>342.39999999999878</v>
+      </c>
+      <c r="C6" s="3">
+        <f>VLOOKUP(A6,population!A4:E35,3)*VLOOKUP(A6,'elec gen per capita'!A5:E24,3)*0.00000001</f>
+        <v>8308.1516437944501</v>
+      </c>
+      <c r="D6" s="3">
+        <f>VLOOKUP(A6,population!A4:E35,4)*VLOOKUP(A6,'elec gen per capita'!A5:E24,4)*0.00000001</f>
+        <v>47041</v>
+      </c>
+      <c r="E6" s="3">
+        <f>VLOOKUP(A6,population!A4:E35,2)*VLOOKUP(A6,'elec gen per capita'!A5:E24,5)*0.00000001</f>
+        <v>98132.999999999534</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>2004</v>
+      </c>
+      <c r="B7" s="3">
+        <f>VLOOKUP(A7,population!A5:E36,5)*VLOOKUP(A7,'elec gen per capita'!A6:E25,2)*0.00000001</f>
+        <v>395.49999999999977</v>
+      </c>
+      <c r="C7" s="3">
+        <f>VLOOKUP(A7,population!A5:E36,3)*VLOOKUP(A7,'elec gen per capita'!A6:E25,3)*0.00000001</f>
+        <v>8260.4271675785712</v>
+      </c>
+      <c r="D7" s="3">
+        <f>VLOOKUP(A7,population!A5:E36,4)*VLOOKUP(A7,'elec gen per capita'!A6:E25,4)*0.00000001</f>
+        <v>47278.999999999942</v>
+      </c>
+      <c r="E7" s="3">
+        <f>VLOOKUP(A7,population!A5:E36,2)*VLOOKUP(A7,'elec gen per capita'!A6:E25,5)*0.00000001</f>
+        <v>104248.99999999932</v>
+      </c>
+      <c r="I7" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7" t="s">
+        <v>12</v>
+      </c>
+      <c r="K7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>2005</v>
+      </c>
+      <c r="B8" s="3">
+        <f>VLOOKUP(A8,population!A6:E37,5)*VLOOKUP(A8,'elec gen per capita'!A7:E26,2)*0.00000001</f>
+        <v>500.49999999999801</v>
+      </c>
+      <c r="C8" s="3">
+        <f>VLOOKUP(A8,population!A6:E37,3)*VLOOKUP(A8,'elec gen per capita'!A7:E26,3)*0.00000001</f>
+        <v>9268.0193973700916</v>
+      </c>
+      <c r="D8" s="3">
+        <f>VLOOKUP(A8,population!A6:E37,4)*VLOOKUP(A8,'elec gen per capita'!A7:E26,4)*0.00000001</f>
+        <v>48601.999999999978</v>
+      </c>
+      <c r="E8" s="3">
+        <f>VLOOKUP(A8,population!A6:E37,2)*VLOOKUP(A8,'elec gen per capita'!A7:E26,5)*0.00000001</f>
+        <v>111689.99999999943</v>
+      </c>
+      <c r="I8">
+        <v>2005</v>
+      </c>
+      <c r="J8">
+        <v>1087</v>
+      </c>
+      <c r="K8">
+        <v>2090</v>
+      </c>
+      <c r="L8">
+        <f>J8+K8</f>
+        <v>3177</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>2006</v>
+      </c>
+      <c r="B9" s="3">
+        <f>VLOOKUP(A9,population!A7:E38,5)*VLOOKUP(A9,'elec gen per capita'!A8:E27,2)*0.00000001</f>
+        <v>345.29999999999717</v>
+      </c>
+      <c r="C9" s="3">
+        <f>VLOOKUP(A9,population!A7:E38,3)*VLOOKUP(A9,'elec gen per capita'!A8:E27,3)*0.00000001</f>
+        <v>10029.143360692491</v>
+      </c>
+      <c r="D9" s="3">
+        <f>VLOOKUP(A9,population!A7:E38,4)*VLOOKUP(A9,'elec gen per capita'!A8:E27,4)*0.00000001</f>
+        <v>50557.999999999942</v>
+      </c>
+      <c r="E9" s="3">
+        <f>VLOOKUP(A9,population!A7:E38,2)*VLOOKUP(A9,'elec gen per capita'!A8:E27,5)*0.00000001</f>
+        <v>118406.99999999996</v>
+      </c>
+      <c r="J9" s="5">
+        <f>J8/L8</f>
+        <v>0.34214667925716086</v>
+      </c>
+      <c r="K9" s="5">
+        <f>K8/L8</f>
+        <v>0.6578533207428392</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>2007</v>
+      </c>
+      <c r="B10" s="3">
+        <f>VLOOKUP(A10,population!A8:E39,5)*VLOOKUP(A10,'elec gen per capita'!A9:E28,2)*0.00000001</f>
+        <v>417.09999999999695</v>
+      </c>
+      <c r="C10" s="3">
+        <f>VLOOKUP(A10,population!A8:E39,3)*VLOOKUP(A10,'elec gen per capita'!A9:E28,3)*0.00000001</f>
+        <v>11609.4933078218</v>
+      </c>
+      <c r="D10" s="3">
+        <f>VLOOKUP(A10,population!A8:E39,4)*VLOOKUP(A10,'elec gen per capita'!A9:E28,4)*0.00000001</f>
+        <v>53791.999999999949</v>
+      </c>
+      <c r="E10" s="3">
+        <f>VLOOKUP(A10,population!A8:E39,2)*VLOOKUP(A10,'elec gen per capita'!A9:E28,5)*0.00000001</f>
+        <v>128128.99999999932</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>2008</v>
+      </c>
+      <c r="B11" s="3">
+        <f>VLOOKUP(A11,population!A9:E40,5)*VLOOKUP(A11,'elec gen per capita'!A10:E29,2)*0.00000001</f>
+        <v>426.59999999999945</v>
+      </c>
+      <c r="C11" s="3">
+        <f>VLOOKUP(A11,population!A9:E40,3)*VLOOKUP(A11,'elec gen per capita'!A10:E29,3)*0.00000001</f>
+        <v>13456.130790738698</v>
+      </c>
+      <c r="D11" s="3">
+        <f>VLOOKUP(A11,population!A9:E40,4)*VLOOKUP(A11,'elec gen per capita'!A10:E29,4)*0.00000001</f>
+        <v>57001.999999999949</v>
+      </c>
+      <c r="E11" s="3">
+        <f>VLOOKUP(A11,population!A9:E40,2)*VLOOKUP(A11,'elec gen per capita'!A10:E29,5)*0.00000001</f>
+        <v>134565.99999999936</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2009</v>
+      </c>
+      <c r="B12" s="3">
+        <f>VLOOKUP(A12,population!A10:E41,5)*VLOOKUP(A12,'elec gen per capita'!A11:E30,2)*0.00000001</f>
+        <v>500.59999999999718</v>
+      </c>
+      <c r="C12" s="3">
+        <f>VLOOKUP(A12,population!A10:E41,3)*VLOOKUP(A12,'elec gen per capita'!A11:E30,3)*0.00000001</f>
+        <v>14887.353807451038</v>
+      </c>
+      <c r="D12" s="3">
+        <f>VLOOKUP(A12,population!A10:E41,4)*VLOOKUP(A12,'elec gen per capita'!A11:E30,4)*0.00000001</f>
+        <v>55007.999999999971</v>
+      </c>
+      <c r="E12" s="3">
+        <f>VLOOKUP(A12,population!A10:E41,2)*VLOOKUP(A12,'elec gen per capita'!A11:E30,5)*0.00000001</f>
+        <v>142689.99999999942</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2010</v>
+      </c>
+      <c r="B13" s="3">
+        <f>VLOOKUP(A13,population!A11:E42,5)*VLOOKUP(A13,'elec gen per capita'!A12:E31,2)*0.00000001</f>
+        <v>473.29999999999728</v>
+      </c>
+      <c r="C13" s="3">
+        <f>VLOOKUP(A13,population!A11:E42,3)*VLOOKUP(A13,'elec gen per capita'!A12:E31,3)*0.00000001</f>
+        <v>15034.503735679122</v>
+      </c>
+      <c r="D13" s="3">
+        <f>VLOOKUP(A13,population!A11:E42,4)*VLOOKUP(A13,'elec gen per capita'!A12:E31,4)*0.00000001</f>
+        <v>58590.999999999971</v>
+      </c>
+      <c r="E13" s="3">
+        <f>VLOOKUP(A13,population!A11:E42,2)*VLOOKUP(A13,'elec gen per capita'!A12:E31,5)*0.00000001</f>
+        <v>150485.99999999956</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>2011</v>
+      </c>
+      <c r="B14" s="3">
+        <f>VLOOKUP(A14,population!A12:E43,5)*VLOOKUP(A14,'elec gen per capita'!A13:E32,2)*0.00000001</f>
+        <v>569.29999999999973</v>
+      </c>
+      <c r="C14" s="3">
+        <f>VLOOKUP(A14,population!A12:E43,3)*VLOOKUP(A14,'elec gen per capita'!A13:E32,3)*0.00000001</f>
+        <v>15593.667055794285</v>
+      </c>
+      <c r="D14" s="3">
+        <f>VLOOKUP(A14,population!A12:E43,4)*VLOOKUP(A14,'elec gen per capita'!A13:E32,4)*0.00000001</f>
+        <v>59678.999999999978</v>
+      </c>
+      <c r="E14" s="3">
+        <f>VLOOKUP(A14,population!A12:E43,2)*VLOOKUP(A14,'elec gen per capita'!A13:E32,5)*0.00000001</f>
+        <v>161161.99999999939</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>2012</v>
+      </c>
+      <c r="B15" s="3">
+        <f>VLOOKUP(A15,population!A13:E44,5)*VLOOKUP(A15,'elec gen per capita'!A14:E33,2)*0.00000001</f>
+        <v>461.1</v>
+      </c>
+      <c r="C15" s="3">
+        <f>VLOOKUP(A15,population!A13:E44,3)*VLOOKUP(A15,'elec gen per capita'!A14:E33,3)*0.00000001</f>
+        <v>15463.380381184088</v>
+      </c>
+      <c r="D15" s="3">
+        <f>VLOOKUP(A15,population!A13:E44,4)*VLOOKUP(A15,'elec gen per capita'!A14:E33,4)*0.00000001</f>
+        <v>63002.999999999935</v>
+      </c>
+      <c r="E15" s="3">
+        <f>VLOOKUP(A15,population!A13:E44,2)*VLOOKUP(A15,'elec gen per capita'!A14:E33,5)*0.00000001</f>
+        <v>164628</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>2013</v>
+      </c>
+      <c r="B16" s="3">
+        <f>VLOOKUP(A16,population!A14:E45,5)*VLOOKUP(A16,'elec gen per capita'!A15:E34,2)*0.00000001</f>
+        <v>536.09999999999934</v>
+      </c>
+      <c r="C16" s="3">
+        <f>VLOOKUP(A16,population!A14:E45,3)*VLOOKUP(A16,'elec gen per capita'!A15:E34,3)*0.00000001</f>
+        <v>17476.12334345654</v>
+      </c>
+      <c r="D16" s="3">
+        <f>VLOOKUP(A16,population!A14:E45,4)*VLOOKUP(A16,'elec gen per capita'!A15:E34,4)*0.00000001</f>
+        <v>61321.999999999978</v>
+      </c>
+      <c r="E16" s="3">
+        <f>VLOOKUP(A16,population!A14:E45,2)*VLOOKUP(A16,'elec gen per capita'!A15:E34,5)*0.00000001</f>
+        <v>168049.99999999994</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>2014</v>
+      </c>
+      <c r="B17" s="3">
+        <f>VLOOKUP(A17,population!A15:E46,5)*VLOOKUP(A17,'elec gen per capita'!A16:E35,2)*0.00000001</f>
+        <v>339.5999999999998</v>
+      </c>
+      <c r="C17" s="3">
+        <f>VLOOKUP(A17,population!A15:E46,3)*VLOOKUP(A17,'elec gen per capita'!A16:E35,3)*0.00000001</f>
+        <v>18073.220891157038</v>
+      </c>
+      <c r="D17" s="3">
+        <f>VLOOKUP(A17,population!A15:E46,4)*VLOOKUP(A17,'elec gen per capita'!A16:E35,4)*0.00000001</f>
+        <v>60812.999999999964</v>
+      </c>
+      <c r="E17" s="3">
+        <f>VLOOKUP(A17,population!A15:E46,2)*VLOOKUP(A17,'elec gen per capita'!A16:E35,5)*0.00000001</f>
+        <v>173551.9999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>2015</v>
+      </c>
+      <c r="B18" s="3">
+        <f>VLOOKUP(A18,population!A16:E47,5)*VLOOKUP(A18,'elec gen per capita'!A17:E36,2)*0.00000001</f>
+        <v>514.69999999999959</v>
+      </c>
+      <c r="C18" s="3">
+        <f>VLOOKUP(A18,population!A16:E47,3)*VLOOKUP(A18,'elec gen per capita'!A17:E36,3)*0.00000001</f>
+        <v>18982.775453888386</v>
+      </c>
+      <c r="D18" s="3">
+        <f>VLOOKUP(A18,population!A16:E47,4)*VLOOKUP(A18,'elec gen per capita'!A17:E36,4)*0.00000001</f>
+        <v>64225.999999999942</v>
+      </c>
+      <c r="E18" s="3">
+        <f>VLOOKUP(A18,population!A16:E47,2)*VLOOKUP(A18,'elec gen per capita'!A17:E36,5)*0.00000001</f>
+        <v>180376.9999999991</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>2016</v>
+      </c>
+      <c r="B19" s="3">
+        <f>VLOOKUP(A19,population!A17:E48,5)*VLOOKUP(A19,'elec gen per capita'!A18:E37,2)*0.00000001</f>
+        <v>537.0999999999982</v>
+      </c>
+      <c r="C19" s="3">
+        <f>VLOOKUP(A19,population!A17:E48,3)*VLOOKUP(A19,'elec gen per capita'!A18:E37,3)*0.00000001</f>
+        <v>19601.778164268497</v>
+      </c>
+      <c r="D19" s="3">
+        <f>VLOOKUP(A19,population!A17:E48,4)*VLOOKUP(A19,'elec gen per capita'!A18:E37,4)*0.00000001</f>
+        <v>66975.999999999956</v>
+      </c>
+      <c r="E19" s="3">
+        <f>VLOOKUP(A19,population!A17:E48,2)*VLOOKUP(A19,'elec gen per capita'!A18:E37,5)*0.00000001</f>
+        <v>191919.99999999965</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>2017</v>
+      </c>
+      <c r="B20" s="3">
+        <f>VLOOKUP(A20,population!A18:E49,5)*VLOOKUP(A20,'elec gen per capita'!A19:E38,2)*0.00000001</f>
+        <v>545.89999999999782</v>
+      </c>
+      <c r="C20" s="3">
+        <f>VLOOKUP(A20,population!A18:E49,3)*VLOOKUP(A20,'elec gen per capita'!A19:E38,3)*0.00000001</f>
+        <v>19431.899999999914</v>
+      </c>
+      <c r="D20" s="3">
+        <f>VLOOKUP(A20,population!A18:E49,4)*VLOOKUP(A20,'elec gen per capita'!A19:E38,4)*0.00000001</f>
+        <v>67674.999999999927</v>
+      </c>
+      <c r="E20" s="3">
+        <f>VLOOKUP(A20,population!A18:E49,2)*VLOOKUP(A20,'elec gen per capita'!A19:E38,5)*0.00000001</f>
+        <v>195149.99999999962</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>2018</v>
+      </c>
+      <c r="B21" s="3">
+        <f>VLOOKUP(A21,population!A19:E50,5)*VLOOKUP(A21,'elec gen per capita'!A20:E39,2)*0.00000001</f>
+        <v>420.39999999999981</v>
+      </c>
+      <c r="C21" s="3">
+        <f>VLOOKUP(A21,population!A19:E50,3)*VLOOKUP(A21,'elec gen per capita'!A20:E39,3)*0.00000001</f>
+        <v>18858.588888999919</v>
+      </c>
+      <c r="D21" s="3">
+        <f>VLOOKUP(A21,population!A19:E50,4)*VLOOKUP(A21,'elec gen per capita'!A20:E39,4)*0.00000001</f>
+        <v>68893</v>
+      </c>
+      <c r="E21" s="3">
+        <f>VLOOKUP(A21,population!A19:E50,2)*VLOOKUP(A21,'elec gen per capita'!A20:E39,5)*0.00000001</f>
+        <v>202837.99999999951</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>2019</v>
+      </c>
+      <c r="B22" s="3">
+        <f>VLOOKUP(A22,population!A20:E51,5)*VLOOKUP(A22,'elec gen per capita'!A21:E40,2)*0.00000001</f>
+        <v>431.09326707939658</v>
+      </c>
+      <c r="C22" s="3">
+        <f>VLOOKUP(A22,population!A20:E51,3)*VLOOKUP(A22,'elec gen per capita'!A21:E40,3)*0.00000001</f>
+        <v>19028.399999999936</v>
+      </c>
+      <c r="D22" s="3">
+        <f>VLOOKUP(A22,population!A20:E51,4)*VLOOKUP(A22,'elec gen per capita'!A21:E40,4)*0.00000001</f>
+        <v>65412.000000000015</v>
+      </c>
+      <c r="E22" s="3">
+        <f>VLOOKUP(A22,population!A20:E51,2)*VLOOKUP(A22,'elec gen per capita'!A21:E40,5)*0.00000001</f>
+        <v>206886.5205694052</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="7">
+        <f>(B22*J9)/MAX($B$22:$E$22)</f>
+        <v>7.12937359937156E-4</v>
+      </c>
+      <c r="C28" s="7">
+        <f>(B22*J9)/MAX($B$22:$D$22)</f>
+        <v>2.2548940527936136E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="7">
+        <f>(B22*K9)/MAX($B$22:$E$22)</f>
+        <v>1.3707811244421861E-3</v>
+      </c>
+      <c r="C29" s="7">
+        <f>(B22*K9)/MAX($B$22:$D$22)</f>
+        <v>4.3355368632370314E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" s="7">
+        <f>C22/MAX($B$22:$E$22)</f>
+        <v>9.1975059310915278E-2</v>
+      </c>
+      <c r="C30" s="7">
+        <f>C22/MAX($B$22:$D$22)</f>
+        <v>0.29090075215556677</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" s="7">
+        <f>D22/MAX($B$22:$E$22)</f>
+        <v>0.31617332932067915</v>
+      </c>
+      <c r="C31" s="7">
+        <f>D22/MAX($B$22:$D$22)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32" s="7">
+        <f>E22/MAX($B$22:$E$22)</f>
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I5" r:id="rId1" xr:uid="{4E453EA0-FFE5-A347-87D2-9D8F447CDF3B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>